<commit_message>
Adding update to backlogs
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossm\Documents\GitHub\Agile_Development_Project1\Product_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAD4895-9C51-F042-B1B6-7F2E85D4A984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC62101-95AB-47B7-B5B7-878552C0F3FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -158,9 +156,6 @@
   </si>
   <si>
     <t>Neja</t>
-  </si>
-  <si>
-    <t>Neja, Kamila</t>
   </si>
   <si>
     <t>27th Jan</t>
@@ -172,6 +167,15 @@
   <si>
     <t>As a programmer, I want the data to be stored in a database 
 so that all the data is easy to access for any user.</t>
+  </si>
+  <si>
+    <t>Stas</t>
+  </si>
+  <si>
+    <t>26th Jan</t>
+  </si>
+  <si>
+    <t>Kamila</t>
   </si>
 </sst>
 </file>
@@ -523,29 +527,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,27 +771,27 @@
   </sheetPr>
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27:K27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
-    <col min="3" max="3" width="84.7109375" customWidth="1"/>
-    <col min="4" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="10" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.54296875" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" customWidth="1"/>
+    <col min="3" max="3" width="84.7265625" customWidth="1"/>
+    <col min="4" max="5" width="25.7265625" customWidth="1"/>
+    <col min="6" max="7" width="8.453125" customWidth="1"/>
+    <col min="8" max="10" width="11.81640625" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="2.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="2.5703125" customWidth="1"/>
-    <col min="15" max="19" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="2.54296875" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" customWidth="1"/>
+    <col min="14" max="14" width="2.54296875" customWidth="1"/>
+    <col min="15" max="19" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -810,7 +814,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -851,13 +855,13 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="8">
         <f t="shared" ref="B3:B25" si="0">ROW()-2</f>
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="9">
@@ -879,7 +883,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="13">
-        <f t="shared" ref="J3:J25" si="1">ROUND((H3/I3),0)</f>
+        <f t="shared" ref="J3:J24" si="1">ROUND((H3/I3),0)</f>
         <v>9</v>
       </c>
       <c r="K3" s="13" t="s">
@@ -894,13 +898,13 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="26" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="9">
@@ -939,13 +943,13 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="27" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="9">
@@ -978,13 +982,13 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="9">
@@ -1017,13 +1021,13 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="9">
@@ -1054,21 +1058,27 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="E8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="13">
         <v>8</v>
       </c>
@@ -1080,7 +1090,7 @@
         <v>8</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L8" s="17"/>
       <c r="M8" s="18"/>
@@ -1091,21 +1101,27 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="27" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="E9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>39</v>
+      </c>
       <c r="H9" s="13">
         <v>8</v>
       </c>
@@ -1117,7 +1133,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L9" s="17"/>
       <c r="M9" s="18"/>
@@ -1128,13 +1144,13 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="9">
@@ -1165,13 +1181,13 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="9">
@@ -1202,13 +1218,13 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="26" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="9">
@@ -1239,13 +1255,13 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="9">
@@ -1276,14 +1292,14 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>42</v>
+      <c r="C14" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
@@ -1313,13 +1329,13 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="9">
@@ -1350,21 +1366,27 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="E16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" s="13">
         <v>3</v>
       </c>
@@ -1376,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L16" s="17"/>
       <c r="M16" s="18"/>
@@ -1387,14 +1409,14 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>41</v>
+      <c r="C17" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
@@ -1424,13 +1446,13 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -1456,13 +1478,13 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -1488,13 +1510,13 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="26" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -1520,13 +1542,13 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="8">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="26" t="s">
         <v>32</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -1552,13 +1574,13 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="9">
@@ -1589,13 +1611,13 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="8">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="29" t="s">
         <v>34</v>
       </c>
       <c r="D23" s="20">
@@ -1626,13 +1648,13 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="8">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="29" t="s">
         <v>35</v>
       </c>
       <c r="D24" s="13">
@@ -1663,23 +1685,23 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="21">
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="21">
@@ -1704,7 +1726,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="4"/>
@@ -1725,18 +1747,18 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="28"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="34"/>
       <c r="L27" s="23"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
@@ -1746,7 +1768,7 @@
       <c r="R27" s="24"/>
       <c r="S27" s="24"/>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="25"/>
@@ -1767,7 +1789,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="25"/>
@@ -1788,7 +1810,7 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
@@ -1809,7 +1831,7 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
@@ -1830,7 +1852,7 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="4"/>
@@ -1851,7 +1873,7 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4"/>
@@ -1872,7 +1894,7 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4"/>
@@ -1893,7 +1915,7 @@
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -1914,7 +1936,7 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4"/>
@@ -1935,7 +1957,7 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4"/>
@@ -1956,7 +1978,7 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4"/>
@@ -1977,7 +1999,7 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4"/>
@@ -1998,7 +2020,7 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4"/>
@@ -2019,7 +2041,7 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4"/>
@@ -2040,7 +2062,7 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4"/>
@@ -2061,7 +2083,7 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="4"/>
@@ -2082,7 +2104,7 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="4"/>
@@ -2103,7 +2125,7 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="4"/>
@@ -2124,7 +2146,7 @@
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
     </row>
-    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="4"/>
@@ -2145,7 +2167,7 @@
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
     </row>
-    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4"/>
@@ -2168,21 +2190,21 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
+          <sortCondition descending="1" ref="H2:H25"/>
+          <sortCondition ref="I2:I25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
           <sortCondition ref="D2:D28"/>
           <sortCondition descending="1" ref="H2:H28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
-          <sortCondition descending="1" ref="H2:H25"/>
-          <sortCondition ref="I2:I25"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>

<commit_message>
Updated data for backlogs
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rossm\Documents\GitHub\Agile_Development_Project1\Product_Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Agile_Development_Project1\Product_Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC62101-95AB-47B7-B5B7-878552C0F3FA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4AF457-5F7D-4DB8-A7DC-C9AEC5DD121D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,14 +24,16 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -176,6 +178,9 @@
   </si>
   <si>
     <t>Kamila</t>
+  </si>
+  <si>
+    <t>Stephen</t>
   </si>
 </sst>
 </file>
@@ -772,8 +777,8 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1161,9 @@
       <c r="D10" s="9">
         <v>1</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="13">
@@ -1341,7 +1348,9 @@
       <c r="D15" s="9">
         <v>1</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="13">
@@ -2190,21 +2199,21 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
+          <sortCondition ref="D2:D28"/>
+          <sortCondition descending="1" ref="H2:H28"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
           <sortCondition descending="1" ref="H2:H25"/>
           <sortCondition ref="I2:I25"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
-          <sortCondition ref="D2:D28"/>
-          <sortCondition descending="1" ref="H2:H28"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>

<commit_message>
Updated Product Backlog files
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Agile_Development_Project1\Product_Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4AF457-5F7D-4DB8-A7DC-C9AEC5DD121D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68891AA5-0664-4346-B2BC-D6B1B9202DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>Stephen</t>
+  </si>
+  <si>
+    <t>Ross</t>
+  </si>
+  <si>
+    <t>Kayla</t>
+  </si>
+  <si>
+    <t>31st Jan</t>
+  </si>
+  <si>
+    <t>28th Jan</t>
   </si>
 </sst>
 </file>
@@ -776,27 +788,27 @@
   </sheetPr>
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="84.7265625" customWidth="1"/>
-    <col min="4" max="5" width="25.7265625" customWidth="1"/>
-    <col min="6" max="7" width="8.453125" customWidth="1"/>
-    <col min="8" max="10" width="11.81640625" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="84.7109375" customWidth="1"/>
+    <col min="4" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="2.54296875" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" customWidth="1"/>
-    <col min="14" max="14" width="2.54296875" customWidth="1"/>
-    <col min="15" max="19" width="8.453125" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="2.5703125" customWidth="1"/>
+    <col min="15" max="19" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -819,7 +831,7 @@
       <c r="R1" s="4"/>
       <c r="S1" s="4"/>
     </row>
-    <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -860,7 +872,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
     </row>
-    <row r="3" spans="1:19" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8">
         <f t="shared" ref="B3:B25" si="0">ROW()-2</f>
@@ -903,7 +915,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="8">
         <f t="shared" si="0"/>
@@ -948,7 +960,7 @@
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="8">
         <f t="shared" si="0"/>
@@ -987,7 +999,7 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="8">
         <f t="shared" si="0"/>
@@ -997,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
@@ -1026,7 +1038,7 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="8">
         <f t="shared" si="0"/>
@@ -1063,7 +1075,7 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="8">
         <f t="shared" si="0"/>
@@ -1106,7 +1118,7 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
         <f t="shared" si="0"/>
@@ -1149,7 +1161,7 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="8">
         <f t="shared" si="0"/>
@@ -1164,8 +1176,12 @@
       <c r="E10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="F10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>36</v>
+      </c>
       <c r="H10" s="13">
         <v>10</v>
       </c>
@@ -1177,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
@@ -1188,7 +1204,7 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
         <f t="shared" si="0"/>
@@ -1225,7 +1241,7 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="8">
         <f t="shared" si="0"/>
@@ -1262,7 +1278,7 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
         <f t="shared" si="0"/>
@@ -1274,9 +1290,15 @@
       <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="E13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="H13" s="13">
         <v>7</v>
       </c>
@@ -1288,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
@@ -1299,7 +1321,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="8">
         <f t="shared" si="0"/>
@@ -1311,9 +1333,15 @@
       <c r="D14" s="9">
         <v>1</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="H14" s="13">
         <v>10</v>
       </c>
@@ -1325,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="18"/>
@@ -1336,7 +1364,7 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
         <f t="shared" si="0"/>
@@ -1351,7 +1379,9 @@
       <c r="E15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="13">
         <v>2</v>
@@ -1364,7 +1394,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
@@ -1375,7 +1405,7 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="8">
         <f t="shared" si="0"/>
@@ -1418,7 +1448,7 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
         <f t="shared" si="0"/>
@@ -1455,7 +1485,7 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="8">
         <f t="shared" si="0"/>
@@ -1487,7 +1517,7 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="8">
         <f t="shared" si="0"/>
@@ -1519,7 +1549,7 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="8">
         <f t="shared" si="0"/>
@@ -1551,7 +1581,7 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="8">
         <f t="shared" si="0"/>
@@ -1583,7 +1613,7 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="8">
         <f t="shared" si="0"/>
@@ -1620,7 +1650,7 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="8">
         <f t="shared" si="0"/>
@@ -1657,7 +1687,7 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="8">
         <f t="shared" si="0"/>
@@ -1669,9 +1699,15 @@
       <c r="D24" s="13">
         <v>1</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="E24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="H24" s="13">
         <v>10</v>
       </c>
@@ -1683,7 +1719,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="1"/>
@@ -1694,7 +1730,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
         <f t="shared" si="0"/>
@@ -1735,7 +1771,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="4"/>
@@ -1756,7 +1792,7 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="22"/>
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
@@ -1777,7 +1813,7 @@
       <c r="R27" s="24"/>
       <c r="S27" s="24"/>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="25"/>
@@ -1798,7 +1834,7 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="25"/>
@@ -1819,7 +1855,7 @@
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
@@ -1840,7 +1876,7 @@
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
@@ -1861,7 +1897,7 @@
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="4"/>
@@ -1882,7 +1918,7 @@
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4"/>
@@ -1903,7 +1939,7 @@
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
     </row>
-    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4"/>
@@ -1924,7 +1960,7 @@
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -1945,7 +1981,7 @@
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4"/>
@@ -1966,7 +2002,7 @@
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4"/>
@@ -1987,7 +2023,7 @@
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
     </row>
-    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4"/>
@@ -2008,7 +2044,7 @@
       <c r="R38" s="4"/>
       <c r="S38" s="4"/>
     </row>
-    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4"/>
@@ -2029,7 +2065,7 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
     </row>
-    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4"/>
@@ -2050,7 +2086,7 @@
       <c r="R40" s="4"/>
       <c r="S40" s="4"/>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4"/>
@@ -2071,7 +2107,7 @@
       <c r="R41" s="4"/>
       <c r="S41" s="4"/>
     </row>
-    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4"/>
@@ -2092,7 +2128,7 @@
       <c r="R42" s="4"/>
       <c r="S42" s="4"/>
     </row>
-    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="4"/>
@@ -2113,7 +2149,7 @@
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
     </row>
-    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="4"/>
@@ -2134,7 +2170,7 @@
       <c r="R44" s="4"/>
       <c r="S44" s="4"/>
     </row>
-    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="4"/>
@@ -2155,7 +2191,7 @@
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
     </row>
-    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="4"/>
@@ -2176,7 +2212,7 @@
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
     </row>
-    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="4"/>
@@ -2199,21 +2235,21 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
+          <sortCondition descending="1" ref="H2:H25"/>
+          <sortCondition ref="I2:I25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
           <sortCondition ref="D2:D28"/>
           <sortCondition descending="1" ref="H2:H28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
-          <sortCondition descending="1" ref="H2:H25"/>
-          <sortCondition ref="I2:I25"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>

<commit_message>
Product and Sprint 2 backlogs updated
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68891AA5-0664-4346-B2BC-D6B1B9202DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB70492C-97D7-434A-B4B7-65B65EFF97FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,15 @@
   </sheets>
   <definedNames>
     <definedName name="Priority">#REF!</definedName>
-    <definedName name="Status">'Agile Product Backlog'!$M$4:$M$23</definedName>
+    <definedName name="Status">'Agile Product Backlog'!$M$4:$M$19</definedName>
     <definedName name="YesNo">#REF!</definedName>
-    <definedName name="Z_89BC23F2_91FE_46D8_B553_D3EF328ABF73_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$B$2:$K$25</definedName>
-    <definedName name="Z_B1AC5159_1992_4676_A928_E62F1FB72277_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$A$2:$S$23</definedName>
+    <definedName name="Z_89BC23F2_91FE_46D8_B553_D3EF328ABF73_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$B$2:$K$24</definedName>
+    <definedName name="Z_B1AC5159_1992_4676_A928_E62F1FB72277_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$A$2:$S$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -91,63 +91,9 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>A user can search based on procedure/condition</t>
-  </si>
-  <si>
-    <t>A user can search based on code</t>
-  </si>
-  <si>
-    <t>A user can search based on live location</t>
-  </si>
-  <si>
-    <t>A user can search based on location input</t>
-  </si>
-  <si>
-    <t>A user can search based on a description of a condition/procedure</t>
-  </si>
-  <si>
-    <t>A user can order the search results based on price</t>
-  </si>
-  <si>
-    <t>A user can order the search results based on distance</t>
-  </si>
-  <si>
-    <t>A user can view the output of a search as a list</t>
-  </si>
-  <si>
-    <t>A user can view the search results on a map</t>
-  </si>
-  <si>
-    <t>A user can see the price information on a placeholder for each result on the map</t>
-  </si>
-  <si>
     <t>As a programmer, I want to find an API to support Google Maps for live location services</t>
   </si>
   <si>
-    <t>A user can set a price range for their search</t>
-  </si>
-  <si>
-    <t>A user can set a distance range for their search</t>
-  </si>
-  <si>
-    <t>The purchaser can delete data from the existing data set</t>
-  </si>
-  <si>
-    <t>The purchaser can load new data from the existing data set</t>
-  </si>
-  <si>
-    <t>The purchaser can update existing data</t>
-  </si>
-  <si>
-    <t>The purchaser can add data to the existing data set</t>
-  </si>
-  <si>
-    <t>A user can navigate with a keyboard</t>
-  </si>
-  <si>
-    <t>A user can view the data regardless of colour blindness</t>
-  </si>
-  <si>
     <t>As a programmer, I would like to create a webpage as the main interface to allow the user easy and effective access to all the data</t>
   </si>
   <si>
@@ -163,14 +109,6 @@
     <t>27th Jan</t>
   </si>
   <si>
-    <t>A user can order the search results based on the ranking 
-which is a combination of price, distance and user feedback.</t>
-  </si>
-  <si>
-    <t>As a programmer, I want the data to be stored in a database 
-so that all the data is easy to access for any user.</t>
-  </si>
-  <si>
     <t>Stas</t>
   </si>
   <si>
@@ -193,13 +131,100 @@
   </si>
   <si>
     <t>28th Jan</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to store longtitude/latitude coordinates for each hospital address in the database a this allows for quicker fetches</t>
+  </si>
+  <si>
+    <t>As a programmer, I would like to optimise a webpage based on user feedback</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to create unit tests for all existing functionality so that I can ensure further development doesn't break any existing code</t>
+  </si>
+  <si>
+    <t>Aa a user, I can search based on code</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on procedure/condition</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on live location</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on location input</t>
+  </si>
+  <si>
+    <t>As a user, I can search based on a description of a procedure/condition</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on price</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on distance</t>
+  </si>
+  <si>
+    <t>As a user, I can view the output of a search as a list</t>
+  </si>
+  <si>
+    <t>As a user, I can view the search results on a map</t>
+  </si>
+  <si>
+    <t>As a user, I can see the price information on a placeholder for each result on the map</t>
+  </si>
+  <si>
+    <t>As a programmer, I want the data to be stored in a database so that all the data is easy to access for any user</t>
+  </si>
+  <si>
+    <t>As a user, I can set a price range for the search</t>
+  </si>
+  <si>
+    <t>As a user, I can set a distance range for the search</t>
+  </si>
+  <si>
+    <t>As a user, I can order the search results based on the ranking which is a combination of price and distance</t>
+  </si>
+  <si>
+    <t>As a user, I can navigate with a keyboard</t>
+  </si>
+  <si>
+    <t>As a user can view the data regardless of colour blindness</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can delete data from the existing data set</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can load new data from the existing data set</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can update existing data</t>
+  </si>
+  <si>
+    <t>As a purchaser, I can add data to the existing data set</t>
+  </si>
+  <si>
+    <t>Neja, Kayla</t>
+  </si>
+  <si>
+    <t>Kamila, Kayla</t>
+  </si>
+  <si>
+    <t>Stas, Stephen</t>
+  </si>
+  <si>
+    <t>Ross, Kamila</t>
+  </si>
+  <si>
+    <t>in Progress</t>
+  </si>
+  <si>
+    <t>3rd Feb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,18 +284,6 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="22"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Century Gothic"/>
       <family val="1"/>
@@ -314,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -458,18 +471,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -534,39 +540,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,11 +777,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O14" sqref="O14"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -875,23 +866,23 @@
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:B25" si="0">ROW()-2</f>
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>17</v>
+        <f t="shared" ref="B3:B28" si="0">ROW()-2</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H3" s="12">
         <v>9</v>
@@ -900,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="13">
-        <f t="shared" ref="J3:J24" si="1">ROUND((H3/I3),0)</f>
+        <f t="shared" ref="J3:J20" si="1">ROUND((H3/I3),0)</f>
         <v>9</v>
       </c>
       <c r="K3" s="13" t="s">
@@ -921,20 +912,20 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>16</v>
+      <c r="C4" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H4" s="13">
         <v>10</v>
@@ -966,24 +957,26 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>18</v>
+      <c r="C5" s="23" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="13">
         <v>7</v>
       </c>
       <c r="I5" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>11</v>
@@ -1005,24 +998,26 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>19</v>
+      <c r="C6" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="D6" s="9">
         <v>2</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I6" s="13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>11</v>
@@ -1044,13 +1039,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>20</v>
+      <c r="C7" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="D7" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="13">
@@ -1081,20 +1078,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="H8" s="13">
         <v>8</v>
@@ -1124,20 +1121,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="F9" s="11" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H9" s="13">
         <v>8</v>
@@ -1167,20 +1164,20 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>23</v>
+      <c r="C10" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H10" s="13">
         <v>10</v>
@@ -1210,27 +1207,31 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>24</v>
+      <c r="C11" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="9">
         <v>2</v>
       </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="G11" s="11"/>
       <c r="H11" s="13">
         <v>5</v>
       </c>
       <c r="I11" s="13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J11" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
@@ -1247,20 +1248,22 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>25</v>
+      <c r="C12" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="13">
         <v>4</v>
       </c>
       <c r="I12" s="13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J12" s="13">
         <f t="shared" si="1"/>
@@ -1284,20 +1287,20 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="F13" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="H13" s="13">
         <v>7</v>
@@ -1327,20 +1330,20 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="31" t="s">
-        <v>41</v>
+      <c r="C14" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H14" s="13">
         <v>10</v>
@@ -1370,17 +1373,17 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>27</v>
+      <c r="C15" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="G15" s="11"/>
       <c r="H15" s="13">
@@ -1411,20 +1414,20 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>28</v>
+      <c r="C16" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="H16" s="13">
         <v>3</v>
@@ -1448,19 +1451,21 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>40</v>
+      <c r="C17" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
       </c>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="13">
@@ -1485,26 +1490,33 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
     </row>
-    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="10"/>
+      <c r="C18" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="13">
-        <v>1</v>
-      </c>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="13">
+        <v>1</v>
+      </c>
+      <c r="J18" s="13">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="K18" s="13" t="s">
         <v>11</v>
       </c>
@@ -1517,26 +1529,33 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
     </row>
-    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="10"/>
+      <c r="C19" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="20">
+        <v>2</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="13">
-        <v>1</v>
-      </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="I19" s="13">
+        <v>2</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="K19" s="13" t="s">
         <v>11</v>
       </c>
@@ -1549,180 +1568,202 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
     </row>
-    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="C20" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="13">
+        <v>1</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="H20" s="13">
-        <v>1</v>
-      </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+        <v>10</v>
+      </c>
+      <c r="I20" s="13">
+        <v>5</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="K20" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="17"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
+        <v>15</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
     </row>
-    <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="8">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
+        <v>14</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>21</v>
+      </c>
       <c r="G21" s="11"/>
-      <c r="H21" s="13">
-        <v>1</v>
-      </c>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="H21" s="21">
+        <v>10</v>
+      </c>
+      <c r="I21" s="21">
+        <v>7</v>
+      </c>
+      <c r="J21" s="13">
+        <f>ROUND((H21/I21),0)</f>
+        <v>1</v>
+      </c>
       <c r="K21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="19"/>
+        <v>12</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="C22" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="21">
         <v>2</v>
       </c>
-      <c r="E22" s="10"/>
+      <c r="E22" s="21" t="s">
+        <v>56</v>
+      </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
-      <c r="H22" s="13">
+      <c r="H22" s="21">
+        <v>4</v>
+      </c>
+      <c r="I22" s="21">
         <v>3</v>
       </c>
-      <c r="I22" s="13">
-        <v>1</v>
-      </c>
       <c r="J22" s="13">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>ROUND((H22/I22),0)</f>
+        <v>1</v>
       </c>
       <c r="K22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="17"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="19"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
     </row>
-    <row r="23" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="8">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="20">
+      <c r="C23" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="21">
         <v>2</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="G23" s="11"/>
-      <c r="H23" s="13">
-        <v>3</v>
-      </c>
-      <c r="I23" s="13">
+      <c r="H23" s="21">
+        <v>8</v>
+      </c>
+      <c r="I23" s="21">
+        <v>5</v>
+      </c>
+      <c r="J23" s="13">
+        <f>ROUND((H23/I23),0)</f>
         <v>2</v>
       </c>
-      <c r="J23" s="13">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
       <c r="K23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="8">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="13">
-        <v>1</v>
+      <c r="C24" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="21">
+        <v>2</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" s="13">
+        <v>55</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="21">
         <v>10</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="21">
         <v>5</v>
       </c>
       <c r="J24" s="13">
-        <f t="shared" si="1"/>
+        <f>ROUND((H24/I24),0)</f>
         <v>2</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L24" s="4"/>
-      <c r="M24" s="1"/>
+      <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
@@ -1730,104 +1771,128 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
     </row>
-    <row r="25" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="21">
-        <v>1</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>39</v>
-      </c>
+      <c r="C25" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="H25" s="21">
-        <v>10</v>
-      </c>
-      <c r="I25" s="21">
-        <v>7</v>
-      </c>
-      <c r="J25" s="13">
-        <f>ROUND((H25/I25),0)</f>
-        <v>1</v>
-      </c>
+      <c r="H25" s="13">
+        <v>1</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="L25" s="17"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="19"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
+      <c r="B26" s="8">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="13">
+        <v>1</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L26" s="17"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="19"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
     </row>
-    <row r="27" spans="1:19" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-    </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="13">
+        <v>1</v>
+      </c>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L27" s="17"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
+      <c r="B28" s="8">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="13">
+        <v>1</v>
+      </c>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="19"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -1837,15 +1902,15 @@
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -1858,7 +1923,6 @@
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2212,29 +2276,17 @@
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
     </row>
-    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
+          <sortCondition ref="D2:D28"/>
+          <sortCondition descending="1" ref="H2:H28"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -2244,21 +2296,9 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
-          <sortCondition ref="D2:D28"/>
-          <sortCondition descending="1" ref="H2:H28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
   </customSheetViews>
-  <mergeCells count="1">
-    <mergeCell ref="B27:K27"/>
-  </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K25" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K17 K18:K28" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updating backlogs and user stories
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Product_Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kamila/Documents/AppliedComp/Agile/Agile_Development_Project1/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB70492C-97D7-434A-B4B7-65B65EFF97FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1209E425-CC43-584C-9731-B149BCB8DC50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -24,16 +24,14 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -218,6 +216,12 @@
   </si>
   <si>
     <t>3rd Feb</t>
+  </si>
+  <si>
+    <t>As a user, I can access the website through a browser</t>
+  </si>
+  <si>
+    <t>Ross, Neja</t>
   </si>
 </sst>
 </file>
@@ -777,11 +781,11 @@
     <tabColor rgb="FFF2F2F2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -866,7 +870,7 @@
     <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:B28" si="0">ROW()-2</f>
+        <f t="shared" ref="B3:B29" si="0">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -1899,21 +1903,38 @@
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="B29" s="8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="13">
+        <v>10</v>
+      </c>
+      <c r="I29" s="13">
+        <v>5</v>
+      </c>
+      <c r="J29" s="13">
+        <v>2</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="17"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="19"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
@@ -1923,6 +1944,7 @@
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1943,7 +1965,6 @@
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2276,8 +2297,38 @@
       <c r="R46" s="4"/>
       <c r="S46" s="4"/>
     </row>
+    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
+          <sortCondition descending="1" ref="H2:H25"/>
+          <sortCondition ref="I2:I25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
@@ -2287,18 +2338,9 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
-          <sortCondition descending="1" ref="H2:H25"/>
-          <sortCondition ref="I2:I25"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
   </customSheetViews>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K17 K18:K28" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K29" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated backlogs Day 4
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kamila/Documents/AppliedComp/Agile/Agile_Development_Project1/Product_Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1209E425-CC43-584C-9731-B149BCB8DC50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F049676-7F43-6C4C-9EAF-49C200597C5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,19 +19,21 @@
     <definedName name="Priority">#REF!</definedName>
     <definedName name="Status">'Agile Product Backlog'!$M$4:$M$19</definedName>
     <definedName name="YesNo">#REF!</definedName>
-    <definedName name="Z_89BC23F2_91FE_46D8_B553_D3EF328ABF73_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$B$2:$K$24</definedName>
+    <definedName name="Z_89BC23F2_91FE_46D8_B553_D3EF328ABF73_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$B$2:$K$25</definedName>
     <definedName name="Z_B1AC5159_1992_4676_A928_E62F1FB72277_.wvu.FilterData" localSheetId="0" hidden="1">'Agile Product Backlog'!$A$2:$S$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -221,7 +223,13 @@
     <t>As a user, I can access the website through a browser</t>
   </si>
   <si>
-    <t>Ross, Neja</t>
+    <t>4th Feb</t>
+  </si>
+  <si>
+    <t>5th Feb</t>
+  </si>
+  <si>
+    <t>6th Feb</t>
   </si>
 </sst>
 </file>
@@ -784,8 +792,8 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K29" sqref="K29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1024,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="16" t="s">
@@ -1052,8 +1060,12 @@
       <c r="E7" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="H7" s="13">
         <v>6</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>3</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
@@ -1261,8 +1273,12 @@
       <c r="E12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="H12" s="13">
         <v>4</v>
       </c>
@@ -1274,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L12" s="17"/>
       <c r="M12" s="18"/>
@@ -1470,7 +1486,9 @@
       <c r="E17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="13">
         <v>4</v>
@@ -1483,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L17" s="17"/>
       <c r="M17" s="18"/>
@@ -1684,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -1736,85 +1754,92 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="8">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="21">
+      <c r="B24" s="8"/>
+      <c r="C24" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="9">
         <v>2</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="21">
+      <c r="E24" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="13">
         <v>10</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="13">
         <v>5</v>
       </c>
       <c r="J24" s="13">
-        <f>ROUND((H24/I24),0)</f>
         <v>2</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-    </row>
-    <row r="25" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+    </row>
+    <row r="25" spans="1:19" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="C25" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="21">
+        <v>2</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="H25" s="13">
-        <v>1</v>
-      </c>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="H25" s="21">
+        <v>10</v>
+      </c>
+      <c r="I25" s="21">
+        <v>5</v>
+      </c>
+      <c r="J25" s="13">
+        <f>ROUND((H25/I25),0)</f>
+        <v>2</v>
+      </c>
       <c r="K25" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="17"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="19"/>
+        <v>12</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
     </row>
-    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="8">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>13</v>
@@ -1846,7 +1871,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>13</v>
@@ -1871,14 +1896,14 @@
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
     </row>
-    <row r="28" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="8">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>13</v>
@@ -1910,25 +1935,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="9">
-        <v>2</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>60</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="13">
-        <v>10</v>
-      </c>
-      <c r="I29" s="13">
-        <v>5</v>
-      </c>
-      <c r="J29" s="13">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="13" t="s">
         <v>11</v>
       </c>
@@ -2320,21 +2339,21 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
+          <sortCondition ref="D2:D28"/>
+          <sortCondition descending="1" ref="H2:H28"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
           <sortCondition descending="1" ref="H2:H25"/>
           <sortCondition ref="I2:I25"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
-          <sortCondition ref="D2:D28"/>
-          <sortCondition descending="1" ref="H2:H28"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>

<commit_message>
Backlog updated at the end of Sprint 2
Product backlog and User stories have been updated to reflect the work finished in Sprint 2
</commit_message>
<xml_diff>
--- a/Product_Backlog/Product Backlog.xlsx
+++ b/Product_Backlog/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejacesnik/Documents/Agile_Development_Project1/Product_Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F049676-7F43-6C4C-9EAF-49C200597C5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E6A5AA-81C8-F44A-9D07-A1992322F541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="640" windowWidth="27840" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -169,9 +169,6 @@
     <t>As a user, I can view the search results on a map</t>
   </si>
   <si>
-    <t>As a user, I can see the price information on a placeholder for each result on the map</t>
-  </si>
-  <si>
     <t>As a programmer, I want the data to be stored in a database so that all the data is easy to access for any user</t>
   </si>
   <si>
@@ -211,18 +208,9 @@
     <t>Stas, Stephen</t>
   </si>
   <si>
-    <t>Ross, Kamila</t>
-  </si>
-  <si>
-    <t>in Progress</t>
-  </si>
-  <si>
     <t>3rd Feb</t>
   </si>
   <si>
-    <t>As a user, I can access the website through a browser</t>
-  </si>
-  <si>
     <t>4th Feb</t>
   </si>
   <si>
@@ -230,6 +218,15 @@
   </si>
   <si>
     <t>6th Feb</t>
+  </si>
+  <si>
+    <t>7th Feb</t>
+  </si>
+  <si>
+    <t>As a programmer, I want to host the website on the server</t>
+  </si>
+  <si>
+    <t>As a user, I can see the price information on a marker for each result on the map</t>
   </si>
 </sst>
 </file>
@@ -792,8 +789,8 @@
   <dimension ref="A1:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -978,7 +975,9 @@
       <c r="E5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>55</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="13">
         <v>7</v>
@@ -991,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="16" t="s">
@@ -1019,8 +1018,12 @@
       <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" s="13">
         <v>8</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>3</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="16" t="s">
@@ -1058,13 +1061,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H7" s="13">
         <v>6</v>
@@ -1233,9 +1236,11 @@
         <v>26</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="11"/>
       <c r="H11" s="13">
         <v>5</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L11" s="17"/>
       <c r="M11" s="18"/>
@@ -1265,19 +1270,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H12" s="13">
         <v>4</v>
@@ -1351,7 +1356,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="9">
         <v>1</v>
@@ -1394,7 +1399,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="9">
         <v>1</v>
@@ -1405,7 +1410,9 @@
       <c r="F15" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="H15" s="13">
         <v>2</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L15" s="17"/>
       <c r="M15" s="18"/>
@@ -1435,7 +1442,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="9">
         <v>1</v>
@@ -1478,7 +1485,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="9">
         <v>2</v>
@@ -1487,7 +1494,7 @@
         <v>20</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G17" s="11"/>
       <c r="H17" s="13">
@@ -1519,16 +1526,20 @@
         <v>16</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="9">
         <v>2</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="H18" s="13">
         <v>3</v>
       </c>
@@ -1540,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="K18" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L18" s="17"/>
       <c r="M18" s="18"/>
@@ -1558,16 +1569,20 @@
         <v>17</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="20">
         <v>2</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="H19" s="13">
         <v>3</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="L19" s="17"/>
       <c r="M19" s="18"/>
@@ -1651,7 +1666,9 @@
       <c r="F21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="H21" s="21">
         <v>10</v>
       </c>
@@ -1663,7 +1680,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -1687,10 +1704,14 @@
         <v>2</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+        <v>24</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="H22" s="21">
         <v>4</v>
       </c>
@@ -1702,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -1729,9 +1750,11 @@
         <v>27</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="11"/>
+        <v>55</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="H23" s="21">
         <v>8</v>
       </c>
@@ -1743,7 +1766,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
@@ -1758,7 +1781,7 @@
       <c r="A24" s="1"/>
       <c r="B24" s="8"/>
       <c r="C24" s="22" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="9">
         <v>2</v>
@@ -1767,10 +1790,10 @@
         <v>20</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H24" s="13">
         <v>10</v>
@@ -1806,10 +1829,14 @@
         <v>2</v>
       </c>
       <c r="E25" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="H25" s="21">
         <v>10</v>
       </c>
@@ -1821,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -1839,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>13</v>
@@ -1871,7 +1898,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>13</v>
@@ -1903,7 +1930,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>13</v>
@@ -1935,7 +1962,7 @@
         <v>27</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>13</v>
@@ -2339,21 +2366,21 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
+        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
+          <sortCondition descending="1" ref="H2:H25"/>
+          <sortCondition ref="I2:I25"/>
+        </sortState>
+      </autoFilter>
+    </customSheetView>
     <customSheetView guid="{89BC23F2-91FE-46D8-B553-D3EF328ABF73}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="B2:K28" xr:uid="{00000000-0000-0000-0000-000000000000}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K28">
           <sortCondition ref="D2:D28"/>
           <sortCondition descending="1" ref="H2:H28"/>
-        </sortState>
-      </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{B1AC5159-1992-4676-A928-E62F1FB72277}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A2:S25" xr:uid="{00000000-0000-0000-0000-000000000000}">
-        <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S25">
-          <sortCondition descending="1" ref="H2:H25"/>
-          <sortCondition ref="I2:I25"/>
         </sortState>
       </autoFilter>
     </customSheetView>

</xml_diff>